<commit_message>
finaliza primeira versao da arvore de busca
</commit_message>
<xml_diff>
--- a/metro.xlsx
+++ b/metro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbf906d5e129b53f/Documentos/Mestrado/Agentes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cbf906d5e129b53f/Documentos/Mestrado/Agentes/metro-a-estrela/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{2095121C-EDD1-4D76-B789-D4F954591ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDBA36D8-414E-4BDA-8604-696AE96DBBBF}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{2095121C-EDD1-4D76-B789-D4F954591ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{030D0AD2-DC79-45EC-B1C8-4C37EF3E50E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1435F0F2-86FA-49CE-9328-6DF29CFE0889}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{1435F0F2-86FA-49CE-9328-6DF29CFE0889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -266,7 +266,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -286,141 +286,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC0C0C0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -762,6 +627,97 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -799,13 +755,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -819,6 +768,57 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC0C0C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -838,24 +838,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{894AFBD2-99FB-45E4-AA31-5E2311FBA504}" name="Tabela2" displayName="Tabela2" ref="A19:O33" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4" headerRowBorderDxfId="17" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{894AFBD2-99FB-45E4-AA31-5E2311FBA504}" name="Tabela2" displayName="Tabela2" ref="A19:O33" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
   <autoFilter ref="A19:O33" xr:uid="{894AFBD2-99FB-45E4-AA31-5E2311FBA504}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{4CB390B5-B673-4944-845D-6AD7839409C4}" name="Coluna1" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{68ADCF1A-7D6F-4988-AAFB-5242CE4DED22}" name="E1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{CF6510D9-ACC6-481C-9EEA-F9C1F0EEF232}" name="E2" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{FE2E0CDF-051C-4814-958E-48A92E2A6104}" name="E3" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{A47C4DD5-E8FE-4B6D-A1EF-9C7A6E303D6B}" name="E4" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{D332DE5B-7E93-41C2-B54E-2D13E83322AF}" name="E5" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{7135C987-AA66-42D5-8111-DD7D88C61ADD}" name="E6" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{EC5496B2-11F1-446B-803A-94B9114883F0}" name="E7" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{071D84F5-6643-4D20-B7D7-C27FC49973D6}" name="E8" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{6D7458E8-F859-4654-8A89-0CF15C7B971D}" name="E9" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{0279583F-C963-4EB0-BF12-08F116686D93}" name="E10" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{EDC94722-DAFF-4AE7-82B2-99EF629F3153}" name="E11" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{5E05E3B2-78BF-4C35-B00E-DCD213AC0FDC}" name="E12" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{E5C92CCB-4D6F-40A2-A0D8-6AA4DC190962}" name="E13" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{01FD1585-2026-4DEE-9BFB-58F5305FB5C8}" name="E14" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{4CB390B5-B673-4944-845D-6AD7839409C4}" name="Coluna1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{68ADCF1A-7D6F-4988-AAFB-5242CE4DED22}" name="E1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{CF6510D9-ACC6-481C-9EEA-F9C1F0EEF232}" name="E2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{FE2E0CDF-051C-4814-958E-48A92E2A6104}" name="E3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A47C4DD5-E8FE-4B6D-A1EF-9C7A6E303D6B}" name="E4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D332DE5B-7E93-41C2-B54E-2D13E83322AF}" name="E5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{7135C987-AA66-42D5-8111-DD7D88C61ADD}" name="E6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EC5496B2-11F1-446B-803A-94B9114883F0}" name="E7" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{071D84F5-6643-4D20-B7D7-C27FC49973D6}" name="E8" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{6D7458E8-F859-4654-8A89-0CF15C7B971D}" name="E9" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{0279583F-C963-4EB0-BF12-08F116686D93}" name="E10" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{EDC94722-DAFF-4AE7-82B2-99EF629F3153}" name="E11" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{5E05E3B2-78BF-4C35-B00E-DCD213AC0FDC}" name="E12" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{E5C92CCB-4D6F-40A2-A0D8-6AA4DC190962}" name="E13" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{01FD1585-2026-4DEE-9BFB-58F5305FB5C8}" name="E14" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1178,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474D45D3-23D0-496A-A652-DC66FFE026FA}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,6 +2304,7 @@
       <c r="N33" s="12"/>
       <c r="O33" s="13"/>
     </row>
+    <row r="35" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>